<commit_message>
pulled in bd values, calculated sedimentation rates and plotted them separately for each lake.
</commit_message>
<xml_diff>
--- a/data/bulk_density_export_from_sent_to_flett_20250602_saved_20250909.xlsx
+++ b/data/bulk_density_export_from_sent_to_flett_20250602_saved_20250909.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliapop/Desktop/SanJuansPaleo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E5B335-863D-5343-B1F7-766B25558AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55B7AFC-0D82-0D4D-B2CB-0C74D8857EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3640" yWindow="760" windowWidth="26600" windowHeight="18880" xr2:uid="{0222E3E0-4977-984D-8BCC-37142D86D7AA}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1247,6 +1247,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3904,7 +3905,7 @@
   <dimension ref="A1:I258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3945,7 +3946,7 @@
       <c r="H1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="14" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>